<commit_message>
day file phan cong len git
</commit_message>
<xml_diff>
--- a/template_task.xlsx
+++ b/template_task.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\capstoneAxios-main\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B2F4199-967B-4B8A-94C8-0CA4D518AE26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3815A056-B57B-4A93-8D35-B10D6A45B787}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,16 +17,6 @@
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
     <ext uri="GoogleSheetsCustomDataVersion1">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataSignature="AMtx7mitsg4nKYzU0T1mG+CZd0js0eHfeQ=="/>
     </ext>
@@ -35,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="23">
   <si>
     <t>Tasks Name</t>
   </si>
@@ -97,10 +87,19 @@
     <t>Cù Thanh Nam</t>
   </si>
   <si>
-    <t>capstoneAxios-main</t>
-  </si>
-  <si>
     <t>Mike Anh Vũ</t>
+  </si>
+  <si>
+    <t>trang Sản Phẩm</t>
+  </si>
+  <si>
+    <t>trang giỏ hàng</t>
+  </si>
+  <si>
+    <t>tạo giao diện trang sản phẩm, tạo 5 api thêm vào 5 sản phẩm trở lên</t>
+  </si>
+  <si>
+    <t>tạo giao diện giỏ hàng, tạo 5 api giỏ hàng và 1 api list sp từ trang sản phẩm</t>
   </si>
 </sst>
 </file>
@@ -181,7 +180,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -292,11 +291,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -359,6 +369,9 @@
     </xf>
     <xf numFmtId="17" fontId="2" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -601,10 +614,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:J986"/>
+  <dimension ref="A1:K986"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" outlineLevelRow="2" x14ac:dyDescent="0.25"/>
@@ -616,11 +629,11 @@
     <col min="7" max="7" width="9.19921875" customWidth="1"/>
     <col min="8" max="8" width="7.59765625" customWidth="1"/>
     <col min="9" max="9" width="8.69921875" customWidth="1"/>
-    <col min="10" max="10" width="33" customWidth="1"/>
+    <col min="10" max="10" width="46.69921875" customWidth="1"/>
     <col min="11" max="26" width="7.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -648,13 +661,14 @@
       <c r="I1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="23" t="s">
         <v>8</v>
       </c>
+      <c r="K1" s="6"/>
     </row>
-    <row r="2" spans="1:10" ht="21.75" customHeight="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="21.75" customHeight="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B2" s="8">
         <v>45675</v>
@@ -666,7 +680,7 @@
         <v>1</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F2" s="8">
         <v>45675</v>
@@ -680,9 +694,11 @@
       <c r="I2" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="12"/>
+      <c r="J2" s="12" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="3" spans="1:10" ht="14.25" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="14.25" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>10</v>
       </c>
@@ -706,7 +722,7 @@
       </c>
       <c r="J3" s="12"/>
     </row>
-    <row r="4" spans="1:10" ht="14.25" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="14.25" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>13</v>
       </c>
@@ -736,7 +752,7 @@
       </c>
       <c r="J4" s="12"/>
     </row>
-    <row r="5" spans="1:10" ht="14.25" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="14.25" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>14</v>
       </c>
@@ -764,7 +780,7 @@
       </c>
       <c r="J5" s="12"/>
     </row>
-    <row r="6" spans="1:10" ht="14.25" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" ht="14.25" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>15</v>
       </c>
@@ -792,7 +808,7 @@
       </c>
       <c r="J6" s="12"/>
     </row>
-    <row r="7" spans="1:10" ht="9" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="9" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>16</v>
       </c>
@@ -820,9 +836,9 @@
       </c>
       <c r="J7" s="19"/>
     </row>
-    <row r="8" spans="1:10" ht="24" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B8" s="8">
         <v>45675</v>
@@ -848,9 +864,11 @@
       <c r="I8" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="J8" s="12"/>
+      <c r="J8" s="12" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="9" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7"/>
       <c r="B9" s="8"/>
       <c r="C9" s="8"/>
@@ -862,7 +880,7 @@
       <c r="I9" s="10"/>
       <c r="J9" s="12"/>
     </row>
-    <row r="10" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7"/>
       <c r="B10" s="8"/>
       <c r="C10" s="8"/>
@@ -874,7 +892,7 @@
       <c r="I10" s="10"/>
       <c r="J10" s="12"/>
     </row>
-    <row r="11" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7"/>
       <c r="B11" s="8"/>
       <c r="C11" s="8"/>
@@ -886,7 +904,7 @@
       <c r="I11" s="10"/>
       <c r="J11" s="12"/>
     </row>
-    <row r="12" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="7"/>
       <c r="B12" s="8"/>
       <c r="C12" s="8"/>
@@ -898,7 +916,7 @@
       <c r="I12" s="10"/>
       <c r="J12" s="12"/>
     </row>
-    <row r="13" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="7"/>
       <c r="B13" s="8"/>
       <c r="C13" s="8"/>
@@ -910,7 +928,7 @@
       <c r="I13" s="10"/>
       <c r="J13" s="12"/>
     </row>
-    <row r="14" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="7"/>
       <c r="B14" s="8"/>
       <c r="C14" s="8"/>
@@ -922,8 +940,8 @@
       <c r="I14" s="10"/>
       <c r="J14" s="12"/>
     </row>
-    <row r="15" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="18" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>